<commit_message>
Added lots of items and blueprints
</commit_message>
<xml_diff>
--- a/AdAstra/Tools Ideas Stats etc.xlsx
+++ b/AdAstra/Tools Ideas Stats etc.xlsx
@@ -12,7 +12,6 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -598,6 +597,27 @@
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -614,27 +634,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -940,7 +939,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:A22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -949,7 +950,7 @@
     <col min="4" max="4" width="34.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="63.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="40.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="26" width="9.140625" style="50"/>
+    <col min="7" max="26" width="9.140625" style="38"/>
     <col min="27" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -974,10 +975,10 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="48" t="s">
         <v>17</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -994,8 +995,8 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="39"/>
-      <c r="B3" s="42"/>
+      <c r="A3" s="46"/>
+      <c r="B3" s="49"/>
       <c r="C3" s="6" t="s">
         <v>39</v>
       </c>
@@ -1010,8 +1011,8 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="39"/>
-      <c r="B4" s="42"/>
+      <c r="A4" s="46"/>
+      <c r="B4" s="49"/>
       <c r="C4" s="6" t="s">
         <v>40</v>
       </c>
@@ -1026,8 +1027,8 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="40"/>
-      <c r="B5" s="43"/>
+      <c r="A5" s="47"/>
+      <c r="B5" s="50"/>
       <c r="C5" s="6"/>
       <c r="D5" s="7" t="s">
         <v>3</v>
@@ -1040,10 +1041,10 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="44" t="s">
+      <c r="A6" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="47" t="s">
+      <c r="B6" s="42" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="13" t="s">
@@ -1060,8 +1061,8 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="45"/>
-      <c r="B7" s="48"/>
+      <c r="A7" s="40"/>
+      <c r="B7" s="43"/>
       <c r="C7" s="25" t="s">
         <v>28</v>
       </c>
@@ -1076,8 +1077,8 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="45"/>
-      <c r="B8" s="48"/>
+      <c r="A8" s="40"/>
+      <c r="B8" s="43"/>
       <c r="C8" s="16" t="s">
         <v>29</v>
       </c>
@@ -1092,8 +1093,8 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="46"/>
-      <c r="B9" s="49"/>
+      <c r="A9" s="41"/>
+      <c r="B9" s="44"/>
       <c r="C9" s="19"/>
       <c r="D9" s="20" t="s">
         <v>3</v>
@@ -1106,10 +1107,10 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="38" t="s">
+      <c r="A10" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="41" t="s">
+      <c r="B10" s="48" t="s">
         <v>22</v>
       </c>
       <c r="C10" s="3" t="s">
@@ -1126,8 +1127,8 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="39"/>
-      <c r="B11" s="42"/>
+      <c r="A11" s="46"/>
+      <c r="B11" s="49"/>
       <c r="C11" s="6"/>
       <c r="D11" s="7" t="s">
         <v>5</v>
@@ -1140,8 +1141,8 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="40"/>
-      <c r="B12" s="43"/>
+      <c r="A12" s="47"/>
+      <c r="B12" s="50"/>
       <c r="C12" s="10"/>
       <c r="D12" s="11" t="s">
         <v>3</v>
@@ -1154,10 +1155,10 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="44" t="s">
+      <c r="A13" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="47" t="s">
+      <c r="B13" s="42" t="s">
         <v>24</v>
       </c>
       <c r="C13" s="13" t="s">
@@ -1174,8 +1175,8 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="45"/>
-      <c r="B14" s="48"/>
+      <c r="A14" s="40"/>
+      <c r="B14" s="43"/>
       <c r="C14" s="16"/>
       <c r="D14" s="17" t="s">
         <v>8</v>
@@ -1188,8 +1189,8 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="45"/>
-      <c r="B15" s="48"/>
+      <c r="A15" s="40"/>
+      <c r="B15" s="43"/>
       <c r="C15" s="16"/>
       <c r="D15" s="17" t="s">
         <v>9</v>
@@ -1200,8 +1201,8 @@
       <c r="F15" s="22"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="45"/>
-      <c r="B16" s="48"/>
+      <c r="A16" s="40"/>
+      <c r="B16" s="43"/>
       <c r="C16" s="16"/>
       <c r="D16" s="17" t="s">
         <v>2</v>
@@ -1212,8 +1213,8 @@
       <c r="F16" s="22"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="45"/>
-      <c r="B17" s="48"/>
+      <c r="A17" s="40"/>
+      <c r="B17" s="43"/>
       <c r="C17" s="16"/>
       <c r="D17" s="17" t="s">
         <v>3</v>
@@ -1226,8 +1227,8 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="46"/>
-      <c r="B18" s="49"/>
+      <c r="A18" s="41"/>
+      <c r="B18" s="44"/>
       <c r="C18" s="19"/>
       <c r="D18" s="20" t="s">
         <v>10</v>
@@ -1238,10 +1239,10 @@
       <c r="F18" s="21"/>
     </row>
     <row r="19" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="38" t="s">
+      <c r="A19" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="B19" s="41" t="s">
+      <c r="B19" s="48" t="s">
         <v>31</v>
       </c>
       <c r="C19" s="3" t="s">
@@ -1256,8 +1257,8 @@
       <c r="F19" s="5"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="39"/>
-      <c r="B20" s="42"/>
+      <c r="A20" s="46"/>
+      <c r="B20" s="49"/>
       <c r="C20" s="6" t="s">
         <v>43</v>
       </c>
@@ -1270,8 +1271,8 @@
       <c r="F20" s="9"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="39"/>
-      <c r="B21" s="42"/>
+      <c r="A21" s="46"/>
+      <c r="B21" s="49"/>
       <c r="C21" s="6"/>
       <c r="D21" s="7" t="s">
         <v>3</v>
@@ -1284,8 +1285,8 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="40"/>
-      <c r="B22" s="43"/>
+      <c r="A22" s="47"/>
+      <c r="B22" s="50"/>
       <c r="C22" s="10"/>
       <c r="D22" s="11" t="s">
         <v>12</v>
@@ -1295,84 +1296,84 @@
       </c>
       <c r="F22" s="12"/>
     </row>
-    <row r="23" spans="1:6" s="50" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:6" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:6" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:6" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:6" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:6" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:6" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:6" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:6" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:6" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="55" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="56" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="57" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="58" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="59" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="60" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="61" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="62" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="63" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="64" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="65" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="66" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="67" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="68" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="69" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="70" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="71" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="72" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="73" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="74" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="75" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="76" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="77" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="78" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="79" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="80" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="81" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="82" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="83" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="84" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="85" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="86" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="87" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="88" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="89" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="90" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="91" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="92" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="93" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="94" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="95" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="96" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="97" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="98" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="99" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="100" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:6" s="38" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:6" s="38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:6" s="38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:6" s="38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:6" s="38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:6" s="38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:6" s="38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:6" s="38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:6" s="38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:6" s="38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" s="38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" s="38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" s="38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" s="38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" s="38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" s="38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" s="38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" s="38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" s="38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" s="38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="55" s="38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="56" s="38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="57" s="38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="58" s="38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="59" s="38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="60" s="38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="61" s="38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="62" s="38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="63" s="38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="64" s="38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="65" s="38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="66" s="38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="67" s="38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="68" s="38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="69" s="38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="70" s="38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="71" s="38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="72" s="38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="73" s="38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="74" s="38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="75" s="38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="76" s="38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="77" s="38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="78" s="38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="79" s="38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="80" s="38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="81" s="38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="82" s="38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="83" s="38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="84" s="38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="85" s="38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="86" s="38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="87" s="38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="88" s="38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="89" s="38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="90" s="38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="91" s="38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="92" s="38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="93" s="38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="94" s="38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="95" s="38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="96" s="38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="97" s="38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="98" s="38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="99" s="38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="100" s="38" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="A13:A18"/>
@@ -1470,69 +1471,69 @@
     </row>
     <row r="13" spans="6:16" x14ac:dyDescent="0.25">
       <c r="I13" s="36">
-        <f>($G$6+1-I12) * $J$9</f>
+        <f t="shared" ref="I13:P13" si="0">($G$6+1-I12) * $J$9</f>
         <v>5.7971014492753624E-2</v>
       </c>
       <c r="J13" s="36">
-        <f>($G$6+1-J12) * $J$9</f>
+        <f t="shared" si="0"/>
         <v>5.0724637681159424E-2</v>
       </c>
       <c r="K13" s="36">
-        <f>($G$6+1-K12) * $J$9</f>
+        <f t="shared" si="0"/>
         <v>4.3478260869565216E-2</v>
       </c>
       <c r="L13" s="36">
-        <f>($G$6+1-L12) * $J$9</f>
+        <f t="shared" si="0"/>
         <v>3.6231884057971016E-2</v>
       </c>
       <c r="M13" s="36">
-        <f>($G$6+1-M12) * $J$9</f>
+        <f t="shared" si="0"/>
         <v>2.8985507246376812E-2</v>
       </c>
       <c r="N13" s="36">
-        <f>($G$6+1-N12) * $J$9</f>
+        <f t="shared" si="0"/>
         <v>2.1739130434782608E-2</v>
       </c>
       <c r="O13" s="36">
-        <f>($G$6+1-O12) * $J$9</f>
+        <f t="shared" si="0"/>
         <v>1.4492753623188406E-2</v>
       </c>
       <c r="P13" s="36">
-        <f>($G$6+1-P12) * $J$9</f>
+        <f t="shared" si="0"/>
         <v>7.246376811594203E-3</v>
       </c>
     </row>
     <row r="14" spans="6:16" x14ac:dyDescent="0.25">
       <c r="I14" s="37">
-        <f>I12*I13</f>
+        <f t="shared" ref="I14:P14" si="1">I12*I13</f>
         <v>0.69565217391304346</v>
       </c>
       <c r="J14" s="37">
-        <f>J12*J13</f>
+        <f t="shared" si="1"/>
         <v>0.65942028985507251</v>
       </c>
       <c r="K14" s="37">
-        <f>K12*K13</f>
+        <f t="shared" si="1"/>
         <v>0.60869565217391308</v>
       </c>
       <c r="L14" s="37">
-        <f>L12*L13</f>
+        <f t="shared" si="1"/>
         <v>0.54347826086956519</v>
       </c>
       <c r="M14" s="37">
-        <f>M12*M13</f>
+        <f t="shared" si="1"/>
         <v>0.46376811594202899</v>
       </c>
       <c r="N14" s="37">
-        <f>N12*N13</f>
+        <f t="shared" si="1"/>
         <v>0.36956521739130432</v>
       </c>
       <c r="O14" s="37">
-        <f>O12*O13</f>
+        <f t="shared" si="1"/>
         <v>0.2608695652173913</v>
       </c>
       <c r="P14" s="37">
-        <f>P12*P13</f>
+        <f t="shared" si="1"/>
         <v>0.13768115942028986</v>
       </c>
     </row>

</xml_diff>